<commit_message>
feat(stats): Actual statistical analysis
</commit_message>
<xml_diff>
--- a/raster-layer-statistics-biblical.xlsx
+++ b/raster-layer-statistics-biblical.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesfulford/Desktop/Harvard Remote Sensing/Final/arabah-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E6BEDA-6D48-584D-97BB-732FB89E5D57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A8A186-2AD5-224F-8E29-CB89D0DE50F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>max</t>
   </si>
@@ -46,40 +47,22 @@
     <t>CHANGE</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>STDEV</t>
-  </si>
-  <si>
-    <t>MEAN</t>
-  </si>
-  <si>
-    <t>GROUP_2_MEAN</t>
-  </si>
-  <si>
-    <t>GROUP_STDEV</t>
-  </si>
-  <si>
-    <t>VARIANCE</t>
-  </si>
-  <si>
-    <t>T_SCORE</t>
-  </si>
-  <si>
-    <t>CONFIDENCE</t>
-  </si>
-  <si>
     <t>Additive Change</t>
-  </si>
-  <si>
-    <t>GROUP_2_STDEV</t>
   </si>
   <si>
     <t>Multiplicative Change</t>
   </si>
   <si>
-    <t>Comparing to fictional group with no change on average for the same number of years. Assuming February mean vegetation index data for this region would be normally distributed if there was no change, for sake of argument.</t>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Mean NDVI</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Relative Difference</t>
   </si>
 </sst>
 </file>
@@ -156,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -166,6 +149,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1568,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1606,30 +1592,14 @@
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -1657,39 +1627,9 @@
         <v>2000</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2">
-        <f>COUNT(J2:J21)</f>
-        <v>19</v>
-      </c>
-      <c r="L2">
-        <f>_xlfn.STDEV.S(J3:J21)</f>
-        <v>455.7959555698863</v>
-      </c>
-      <c r="M2">
-        <f>AVERAGE(J3:J21)</f>
-        <v>18.229149797570916</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <f>L2</f>
-        <v>455.7959555698863</v>
-      </c>
-      <c r="P2">
-        <f>SQRT((POWER(L2, 2)/K2) + (POWER(O2, 2)/K2))</f>
-        <v>147.87973531640171</v>
-      </c>
-      <c r="Q2">
-        <f>ABS(M2-N2)/P2</f>
-        <v>0.12327010025118076</v>
-      </c>
-      <c r="R2" s="3">
-        <f>_xlfn.T.DIST(Q2,K2-2,TRUE)</f>
-        <v>0.54833055381381679</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="R2" s="3"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1720,9 +1660,6 @@
         <f>C3-C2</f>
         <v>308.59076923076918</v>
       </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -2268,75 +2205,26 @@
       <c r="J23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K24">
-        <f>COUNT(J24:J43)</f>
-        <v>19</v>
-      </c>
-      <c r="L24">
-        <f>_xlfn.STDEV.S(J25:J43)</f>
-        <v>0.14948404469897122</v>
-      </c>
-      <c r="M24">
-        <f>AVERAGE(J25:J43)</f>
-        <v>1.0043741127641115</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="O24">
-        <f>L24</f>
-        <v>0.14948404469897122</v>
-      </c>
-      <c r="P24">
-        <f>SQRT((POWER(L24, 2)/K24) + (POWER(O24, 2)/K24))</f>
-        <v>4.8499028334883086E-2</v>
-      </c>
-      <c r="Q24">
-        <f>ABS(M24-N24)/P24</f>
-        <v>9.0189698933934859E-2</v>
-      </c>
-      <c r="R24" s="3">
-        <f>_xlfn.T.DIST(Q24,K24-2,TRUE)</f>
-        <v>0.53540470901535653</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="R24" s="3"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J25" s="3">
         <f>C2/C3</f>
         <v>0.8989702809918021</v>
       </c>
-      <c r="N25" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J26" s="3">
@@ -2450,4 +2338,360 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA94AEF9-51EF-ED4C-9881-22F42C134F78}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2745.8646153846148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2001</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3054.455384615384</v>
+      </c>
+      <c r="C3" s="5">
+        <f>B3-B2</f>
+        <v>308.59076923076918</v>
+      </c>
+      <c r="D3" s="6">
+        <f>C3/B2</f>
+        <v>0.1123838252992472</v>
+      </c>
+      <c r="F3" s="7">
+        <f>AVERAGE(C3:C21)</f>
+        <v>18.229149797570916</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2002</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3558.9092307692308</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" ref="C4:C21" si="0">B4-B3</f>
+        <v>504.45384615384683</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" ref="D4:D21" si="1">C4/B3</f>
+        <v>0.16515345049551852</v>
+      </c>
+      <c r="F4">
+        <f>_xlfn.STDEV.S(C3:C21)</f>
+        <v>455.7959555698863</v>
+      </c>
+      <c r="G4">
+        <f>F3/F4</f>
+        <v>3.9994101691356219E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2003</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3723.956923076923</v>
+      </c>
+      <c r="C5" s="5">
+        <f t="shared" si="0"/>
+        <v>165.04769230769216</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="1"/>
+        <v>4.6375920712093684E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2004</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2871.5907692307692</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" si="0"/>
+        <v>-852.36615384615379</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.22888722169801187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2005</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3228.8830769230772</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="0"/>
+        <v>357.29230769230799</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.12442312864378587</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2006</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3156.752307692308</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="0"/>
+        <v>-72.130769230769147</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="1"/>
+        <v>-2.2339232332780918E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2007</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3133.476923076923</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="0"/>
+        <v>-23.275384615385065</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="1"/>
+        <v>-7.3732058605510782E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2008</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2819.1323076923081</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="0"/>
+        <v>-314.34461538461483</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.10031815235962982</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2009</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2559.4907692307688</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>-259.64153846153931</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" si="1"/>
+        <v>-9.2099805941381049E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2745.8646153846148</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>186.37384615384599</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="1"/>
+        <v>7.2816768239355248E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2011</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2454.5061538461541</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="0"/>
+        <v>-291.35846153846069</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.10610809429788655</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2012</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2678.2415384615379</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="0"/>
+        <v>223.73538461538374</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="1"/>
+        <v>9.1152912476831882E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15" s="5">
+        <v>3092.104615384615</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="0"/>
+        <v>413.86307692307719</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="1"/>
+        <v>0.15452791355062492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2014</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2581.4907692307688</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="0"/>
+        <v>-510.61384615384623</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.16513472526553988</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2015</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3574.941538461539</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="0"/>
+        <v>993.45076923077022</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="1"/>
+        <v>0.38483607265688502</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2016</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2973.3876923076919</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="0"/>
+        <v>-601.55384615384719</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.16826956180456124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2017</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2865.6569230769228</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="0"/>
+        <v>-107.73076923076906</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" si="1"/>
+        <v>-3.6231659096953334E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2018</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2557.666153846154</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="0"/>
+        <v>-307.99076923076882</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.10747649753553609</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2019</v>
+      </c>
+      <c r="B21" s="5">
+        <v>3092.2184615384622</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="0"/>
+        <v>534.5523076923082</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="1"/>
+        <v>0.20900003188002542</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>